<commit_message>
- Matrix updated - Updated Shapes
</commit_message>
<xml_diff>
--- a/Documents/Helios Matrix.xlsx
+++ b/Documents/Helios Matrix.xlsx
@@ -2638,7 +2638,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4063,7 +4063,9 @@
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5">
+        <v>5</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>

</xml_diff>

<commit_message>
Updated:  -Decks - Blockout map - PointIncrease - Influence Data - Matrix
</commit_message>
<xml_diff>
--- a/Documents/Helios Matrix.xlsx
+++ b/Documents/Helios Matrix.xlsx
@@ -2282,9 +2282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S19" sqref="S19"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,8 +2414,12 @@
       <c r="C2" s="8">
         <v>-30</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
       <c r="F2" s="5">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
- Updated Decks & Matrix
</commit_message>
<xml_diff>
--- a/Documents/Helios Matrix.xlsx
+++ b/Documents/Helios Matrix.xlsx
@@ -2282,9 +2282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB3" s="15"/>
     </row>

</xml_diff>

<commit_message>
- Updated Colliders - Updated Decks - Balancing update
</commit_message>
<xml_diff>
--- a/Documents/Helios Matrix.xlsx
+++ b/Documents/Helios Matrix.xlsx
@@ -2284,7 +2284,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
+      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2657,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -2711,7 +2711,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="5">
         <v>15</v>
@@ -2779,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
@@ -2825,7 +2825,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
@@ -2871,7 +2871,7 @@
         <v>-5</v>
       </c>
       <c r="P10" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -2912,7 +2912,9 @@
       <c r="M11" s="5">
         <v>5</v>
       </c>
-      <c r="N11" s="5"/>
+      <c r="N11" s="5">
+        <v>5</v>
+      </c>
       <c r="O11" s="5">
         <v>5</v>
       </c>
@@ -3165,7 +3167,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="4">
         <v>-15</v>
@@ -3188,7 +3190,7 @@
       </c>
       <c r="AB16" s="15"/>
     </row>
-    <row r="17" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
@@ -3209,10 +3211,10 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R17" s="4">
         <v>2</v>

</xml_diff>